<commit_message>
Unit testing done for correlation and correlation square
</commit_message>
<xml_diff>
--- a/TP01/documents/Tableau de cas de tests.xlsx
+++ b/TP01/documents/Tableau de cas de tests.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="516" yWindow="516" windowWidth="15996" windowHeight="7356"/>
+    <workbookView xWindow="510" yWindow="510" windowWidth="15990" windowHeight="7350"/>
   </bookViews>
   <sheets>
     <sheet name="Registre de tests" sheetId="1" r:id="rId1"/>
@@ -481,16 +481,16 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="72.88671875" customWidth="1"/>
-    <col min="4" max="4" width="18.44140625" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="72.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1">
@@ -527,7 +527,7 @@
         <v>11</v>
       </c>
       <c r="E2" s="2" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>2</v>
@@ -546,8 +546,8 @@
       <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="b">
-        <v>0</v>
+      <c r="E3" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>2</v>
@@ -566,7 +566,7 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="b">
+      <c r="E4" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -586,8 +586,8 @@
       <c r="D5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E5" t="b">
-        <v>0</v>
+      <c r="E5" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>2</v>
@@ -606,8 +606,8 @@
       <c r="D6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E6" t="b">
-        <v>0</v>
+      <c r="E6" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>2</v>
@@ -626,7 +626,7 @@
       <c r="D7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E7" t="b">
+      <c r="E7" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -646,8 +646,8 @@
       <c r="D8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E8" t="b">
-        <v>0</v>
+      <c r="E8" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>2</v>
@@ -666,8 +666,8 @@
       <c r="D9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E9" t="b">
-        <v>0</v>
+      <c r="E9" s="2" t="b">
+        <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>2</v>
@@ -686,7 +686,7 @@
       <c r="D10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E10" t="b">
+      <c r="E10" s="2" t="b">
         <v>0</v>
       </c>
       <c r="F10" s="2" t="s">
@@ -735,13 +735,13 @@
       <c r="D16" s="2"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:1" ht="13.2">
+    <row r="17" spans="1:1" ht="12.75">
       <c r="A17" s="2"/>
     </row>
-    <row r="18" spans="1:1" ht="13.2">
+    <row r="18" spans="1:1" ht="12.75">
       <c r="A18" s="2"/>
     </row>
-    <row r="19" spans="1:1" ht="13.2">
+    <row r="19" spans="1:1" ht="12.75">
       <c r="A19" s="2"/>
     </row>
   </sheetData>
@@ -773,7 +773,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1">
       <c r="A1" s="2" t="s">
@@ -812,9 +812,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="29.33203125" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1">

</xml_diff>